<commit_message>
minor fixes before first submission
</commit_message>
<xml_diff>
--- a/final_analyses/data/characteristics_data-extraction-table.xlsx
+++ b/final_analyses/data/characteristics_data-extraction-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Coding/projects/tocilizumab_reanalysis/final_analyses/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639E2612-892D-EE4D-9CF9-30FB9709F25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84F6417-F48A-5440-B056-1030D6B70033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" xr2:uid="{7DAF0226-96AB-5B4B-8F8E-0559262C285F}"/>
+    <workbookView xWindow="-1260" yWindow="-17140" windowWidth="28800" windowHeight="17140" xr2:uid="{7DAF0226-96AB-5B4B-8F8E-0559262C285F}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>trial</t>
   </si>
@@ -124,9 +124,6 @@
     <t>EMPACTA</t>
   </si>
   <si>
-    <t>Salvarini</t>
-  </si>
-  <si>
     <t>Stone</t>
   </si>
   <si>
@@ -239,6 +236,27 @@
   </si>
   <si>
     <t>64 (14)</t>
+  </si>
+  <si>
+    <t>dose_toci</t>
+  </si>
+  <si>
+    <t>8 mg/kg (maximum 800 mg), followed by a second infusion 8 to 24 hours after the first at physician discretion</t>
+  </si>
+  <si>
+    <t>8 mg/kg (maximum 800 mg), followed by a second infusion 12 to 24 hours after the first at physician discretion</t>
+  </si>
+  <si>
+    <t>From 8mg/kg if bodyweight ≤40 kg to 800mg if bodyweight &gt;90kg, followed by a second infusion 12 to 24 hours after the first at physician discretion</t>
+  </si>
+  <si>
+    <t>8 mg/kg, followed by 400 mg infusion on day 3 at physician discretion</t>
+  </si>
+  <si>
+    <t>8 mg/kg (maximum of 800 mg), followed by a second dose after 12 hours</t>
+  </si>
+  <si>
+    <t>Salvarani</t>
   </si>
 </sst>
 </file>
@@ -592,25 +610,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41467D1-F3B6-BE45-80E1-808CE70470D6}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,126 +640,132 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" t="s">
-        <v>43</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>2021</v>
       </c>
       <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2">
+        <v>66</v>
+      </c>
+      <c r="H2">
+        <v>69</v>
+      </c>
+      <c r="I2">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2">
-        <v>66</v>
-      </c>
-      <c r="G2">
-        <v>69</v>
-      </c>
-      <c r="H2">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0.82</v>
       </c>
       <c r="K2" s="1">
         <v>0.82</v>
       </c>
       <c r="L2" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="M2" s="1">
         <v>0.95</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>0.96</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>0.46</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>0.41</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>0.13</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>0.45</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>0.41</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>2022</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>2094</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -748,64 +773,67 @@
         <v>2021</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3">
+        <v>74</v>
+      </c>
+      <c r="H3">
+        <v>70</v>
+      </c>
+      <c r="I3">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>50</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3">
-        <v>74</v>
-      </c>
-      <c r="G3">
-        <v>70</v>
-      </c>
-      <c r="H3">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.8</v>
       </c>
       <c r="K3" s="1">
         <v>0.8</v>
       </c>
       <c r="L3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="1">
         <v>0.82</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>0.85</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.01</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>0.71</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.01</v>
       </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
         <v>0.69</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>0.3</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>353</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -813,65 +841,68 @@
         <v>2021</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4">
-        <v>70</v>
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
       </c>
       <c r="G4">
         <v>70</v>
       </c>
       <c r="H4">
+        <v>70</v>
+      </c>
+      <c r="I4">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="1">
         <v>0.19</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>0.28499999999999998</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
         <v>0.26500000000000001</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>0.32</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>0.38</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="R4" s="1">
         <v>0.31</v>
       </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
         <v>0.27</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>0.38</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>294</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>144</v>
       </c>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -879,125 +910,131 @@
         <v>2020</v>
       </c>
       <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5">
+        <v>70</v>
+      </c>
+      <c r="H5">
+        <v>66</v>
+      </c>
+      <c r="I5">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5">
-        <v>70</v>
-      </c>
-      <c r="G5">
-        <v>66</v>
-      </c>
-      <c r="H5">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>0.33</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>0.61</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>0.89</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>0.9</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
       </c>
       <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
         <v>1</v>
-      </c>
-      <c r="R5" s="1">
-        <v>0</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <v>63</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B6">
         <v>2020</v>
       </c>
       <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6">
+        <v>67</v>
+      </c>
+      <c r="H6">
+        <v>56</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
         <v>50</v>
       </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6">
-        <v>67</v>
-      </c>
-      <c r="G6">
-        <v>56</v>
-      </c>
-      <c r="H6">
-        <v>30</v>
-      </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>0.1</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>0.11</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
       </c>
       <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="O6" s="1">
+      <c r="P6" s="1">
         <v>1</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
       </c>
       <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>0</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>60</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>62</v>
       </c>
     </row>
@@ -1046,43 +1083,43 @@
           <x14:formula1>
             <xm:f>data_validation!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
+          <xm:sqref>I1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2BC15148-1141-0A44-9A42-0D9E07BA9397}">
           <x14:formula1>
             <xm:f>data_validation!$G$2:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AC298B7D-15CD-1046-BC10-13123BF8AA42}">
           <x14:formula1>
             <xm:f>data_validation!$G$1</xm:f>
           </x14:formula1>
-          <xm:sqref>I1</xm:sqref>
+          <xm:sqref>J1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7718277E-225A-B34E-A942-935E96A2E371}">
           <x14:formula1>
             <xm:f>data_validation!$H$1</xm:f>
           </x14:formula1>
-          <xm:sqref>J1</xm:sqref>
+          <xm:sqref>K1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEB81643-8E7A-834B-9016-9AC851F649F9}">
           <x14:formula1>
             <xm:f>data_validation!$I$1</xm:f>
           </x14:formula1>
-          <xm:sqref>K1</xm:sqref>
+          <xm:sqref>L1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0204BDE4-9CCC-9B47-9A83-EFFA30998C39}">
           <x14:formula1>
             <xm:f>data_validation!$J$1</xm:f>
           </x14:formula1>
-          <xm:sqref>L1</xm:sqref>
+          <xm:sqref>M1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{66A9D08F-970B-7949-BF04-145E8367BCA8}">
           <x14:formula1>
             <xm:f>data_validation!$K$1</xm:f>
           </x14:formula1>
-          <xm:sqref>M1</xm:sqref>
+          <xm:sqref>N1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1210,7 +1247,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,10 +1291,10 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
         <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1268,10 +1305,10 @@
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1282,10 +1319,10 @@
         <v>2021</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1293,10 +1330,10 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1304,33 +1341,33 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>